<commit_message>
Se modificó el diseño de la tabla basado en los campos del de calculo de nomina del excel
</commit_message>
<xml_diff>
--- a/ERPSEI/wwwroot/templates/PlantillaAsistencia.xlsx
+++ b/ERPSEI/wwwroot/templates/PlantillaAsistencia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Cruz\source\repos\ERPSEI\ERPSEI\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E407B30-121C-4544-A90B-D3379ED5D36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE17671E-52A6-4573-935D-0FDDAF784DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6762AA26-D02E-40A8-A0E1-8D8B1472EB0A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Asistencia" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Asistencia!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Asistencia!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,30 +39,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>ID EMPLEADO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>NOMBRE</t>
   </si>
   <si>
-    <t>FECHA HORA</t>
-  </si>
-  <si>
     <t>FECHA</t>
   </si>
   <si>
     <t>HORA</t>
   </si>
   <si>
-    <t>DIRECCION</t>
-  </si>
-  <si>
-    <t>NOMBRE DISPOSITIVO</t>
-  </si>
-  <si>
-    <t>SERIAL DISPOSITIVO</t>
+    <t>HORARIO</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>FECHA Y HORA</t>
   </si>
 </sst>
 </file>
@@ -451,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F61039-1970-47A9-8472-075D13B3C46B}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,38 +459,30 @@
     <col min="4" max="4" width="15.109375" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="14.88671875" customWidth="1"/>
-    <col min="7" max="7" width="37.44140625" customWidth="1"/>
-    <col min="8" max="8" width="42.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{92F61039-1970-47A9-8472-075D13B3C46B}"/>
+  <autoFilter ref="A1:F1" xr:uid="{92F61039-1970-47A9-8472-075D13B3C46B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se cambió la plantilla de asistencia y se habilito la exportacion de asistencias basado en el compilado de datos
</commit_message>
<xml_diff>
--- a/ERPSEI/wwwroot/templates/PlantillaAsistencia.xlsx
+++ b/ERPSEI/wwwroot/templates/PlantillaAsistencia.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Cruz\source\repos\ERPSEI\ERPSEI\wwwroot\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge Cruz\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE17671E-52A6-4573-935D-0FDDAF784DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8001212-1BE0-45CA-867F-E51899544CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6762AA26-D02E-40A8-A0E1-8D8B1472EB0A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Asistencia" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Asistencia!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Asistencia!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,24 +39,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>NOMBRE</t>
+    <t>ID Empleado</t>
   </si>
   <si>
-    <t>FECHA</t>
+    <t>Nombre</t>
   </si>
   <si>
-    <t>HORA</t>
-  </si>
-  <si>
-    <t>HORARIO</t>
-  </si>
-  <si>
-    <t>DIA</t>
-  </si>
-  <si>
-    <t>FECHA Y HORA</t>
+    <t>Fecha/Hora</t>
   </si>
 </sst>
 </file>
@@ -445,44 +436,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F61039-1970-47A9-8472-075D13B3C46B}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
     <col min="2" max="2" width="45.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.21875" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{92F61039-1970-47A9-8472-075D13B3C46B}"/>
+  <autoFilter ref="A1:C1" xr:uid="{92F61039-1970-47A9-8472-075D13B3C46B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>